<commit_message>
rounding and scaling adjustments
</commit_message>
<xml_diff>
--- a/Data/Electricity Storage.xlsx
+++ b/Data/Electricity Storage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emirsener/Desktop/Benders-Decomposition/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8603415D-176B-6941-A030-BBD935C79133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603D63B9-AAEB-EE4A-ABD1-C32B0CEAC38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20060" xr2:uid="{EDF38AB8-B67A-6545-84A8-C231FAB8949A}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20060" xr2:uid="{EDF38AB8-B67A-6545-84A8-C231FAB8949A}"/>
   </bookViews>
   <sheets>
     <sheet name="Initial values" sheetId="7" r:id="rId1"/>
@@ -146,11 +146,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +467,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -489,8 +488,8 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <f>350/0.9</f>
-        <v>388.88888888888886</v>
+        <f>350*1000/0.9</f>
+        <v>388888.88888888888</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -544,8 +543,8 @@
         <v>17</v>
       </c>
       <c r="B8">
-        <f>ROUND(0.03/0.9,4)</f>
-        <v>3.3300000000000003E-2</v>
+        <f>ROUND(0.03*1000/0.9,4)</f>
+        <v>33.333300000000001</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -561,7 +560,7 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -847,7 +846,7 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5">
         <f>ROUND(EXP(-B3),4)</f>
         <v>0.4803</v>
       </c>

</xml_diff>